<commit_message>
Refactor the now noise indicator to be a signal noise score (same value different name
</commit_message>
<xml_diff>
--- a/measured.xlsx
+++ b/measured.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="amateur" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="porn" sheetId="4" r:id="rId4"/>
     <sheet name="products" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -34,9 +34,6 @@
     <t>We have the right label in the output (something specific enough to identify the main subject)</t>
   </si>
   <si>
-    <t>Low noise</t>
-  </si>
-  <si>
     <t>We don't have wrong labels (too generic terms don't count)</t>
   </si>
   <si>
@@ -356,13 +353,16 @@
   </si>
   <si>
     <t>malinshopper-wine</t>
+  </si>
+  <si>
+    <t>Signal / noise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -374,6 +374,18 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -394,8 +406,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -409,7 +423,9 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -741,9 +757,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C19" sqref="C19"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -776,11 +792,11 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -800,44 +816,44 @@
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>3</v>
+      <c r="E6" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>3</v>
+      <c r="G6" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -860,7 +876,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -883,7 +899,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
         <v>3</v>
@@ -906,7 +922,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
@@ -929,7 +945,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
@@ -952,7 +968,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="3">
         <v>4</v>
@@ -975,7 +991,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3">
         <v>4</v>
@@ -998,7 +1014,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
@@ -1021,7 +1037,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3">
         <v>4</v>
@@ -1044,7 +1060,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -1067,7 +1083,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="3">
         <v>4</v>
@@ -1090,7 +1106,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="3">
         <v>0</v>
@@ -1113,7 +1129,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -1136,7 +1152,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="3">
         <v>5</v>
@@ -1159,7 +1175,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="3">
         <v>3</v>
@@ -1182,7 +1198,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="3">
         <v>4</v>
@@ -1205,7 +1221,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="3">
         <v>3</v>
@@ -1228,7 +1244,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -1251,7 +1267,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
@@ -1274,7 +1290,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="3">
         <v>3</v>
@@ -1297,6 +1313,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1311,7 +1328,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1344,11 +1361,11 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1368,44 +1385,44 @@
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
+      <c r="C6" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>3</v>
+      <c r="E6" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>3</v>
+      <c r="G6" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
@@ -1428,7 +1445,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -1451,7 +1468,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
@@ -1474,7 +1491,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
@@ -1497,7 +1514,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -1520,7 +1537,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -1543,7 +1560,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -1566,7 +1583,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -1589,7 +1606,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
@@ -1612,7 +1629,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3">
         <v>3</v>
@@ -1635,7 +1652,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3">
         <v>4</v>
@@ -1658,7 +1675,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3">
         <v>2</v>
@@ -1681,7 +1698,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -1704,7 +1721,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -1727,7 +1744,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -1750,7 +1767,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="3">
         <v>4</v>
@@ -1773,7 +1790,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -1796,7 +1813,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
@@ -1819,7 +1836,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="3">
         <v>4</v>
@@ -1842,7 +1859,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3">
         <v>2</v>
@@ -1888,7 +1905,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1921,11 +1938,11 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1945,44 +1962,44 @@
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
+      <c r="C6" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>3</v>
+      <c r="E6" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>3</v>
+      <c r="G6" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
@@ -2005,7 +2022,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -2028,7 +2045,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3">
         <v>5</v>
@@ -2051,7 +2068,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3">
         <v>5</v>
@@ -2074,7 +2091,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3">
         <v>4</v>
@@ -2097,7 +2114,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -2120,7 +2137,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -2143,7 +2160,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -2166,7 +2183,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3">
         <v>4</v>
@@ -2189,7 +2206,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>4</v>
@@ -2212,7 +2229,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3">
         <v>3</v>
@@ -2235,7 +2252,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="3">
         <v>4</v>
@@ -2258,7 +2275,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="3">
         <v>4</v>
@@ -2281,7 +2298,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
@@ -2304,7 +2321,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -2327,7 +2344,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
@@ -2350,7 +2367,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="3">
         <v>4</v>
@@ -2373,7 +2390,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
@@ -2396,7 +2413,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3">
         <v>4</v>
@@ -2419,7 +2436,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="3">
         <v>0</v>
@@ -2465,7 +2482,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2502,11 +2519,11 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2530,55 +2547,55 @@
     <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
+      <c r="C6" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>3</v>
+      <c r="F6" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>3</v>
+      <c r="I6" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -2587,7 +2604,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
@@ -2610,7 +2627,7 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -2619,7 +2636,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="3">
         <v>3</v>
@@ -2642,7 +2659,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
@@ -2651,7 +2668,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="3">
         <v>2</v>
@@ -2674,7 +2691,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="3">
         <v>2</v>
@@ -2683,7 +2700,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="3">
         <v>2</v>
@@ -2706,7 +2723,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
@@ -2715,7 +2732,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="3">
         <v>3</v>
@@ -2738,7 +2755,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -2747,7 +2764,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="3">
         <v>4</v>
@@ -2770,7 +2787,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -2779,7 +2796,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="3">
         <v>4</v>
@@ -2802,7 +2819,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -2811,7 +2828,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
@@ -2834,7 +2851,7 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="3">
         <v>3</v>
@@ -2843,7 +2860,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="3">
         <v>3</v>
@@ -2866,7 +2883,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3">
         <v>3</v>
@@ -2875,7 +2892,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="3">
         <v>3</v>
@@ -2898,7 +2915,7 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -2907,7 +2924,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="3">
         <v>2</v>
@@ -2930,7 +2947,7 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="3">
         <v>2</v>
@@ -2939,7 +2956,7 @@
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="3">
         <v>4</v>
@@ -2962,7 +2979,7 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" s="3">
         <v>3</v>
@@ -2971,7 +2988,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="3">
         <v>3</v>
@@ -2994,7 +3011,7 @@
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="3">
         <v>2</v>
@@ -3003,7 +3020,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E20" s="3">
         <v>3</v>
@@ -3026,7 +3043,7 @@
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="3">
         <v>4</v>
@@ -3035,7 +3052,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="3">
         <v>4</v>
@@ -3058,7 +3075,7 @@
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="3">
         <v>4</v>
@@ -3067,7 +3084,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
@@ -3090,7 +3107,7 @@
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
@@ -3099,7 +3116,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="3">
         <v>2</v>
@@ -3122,7 +3139,7 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="3">
         <v>3</v>
@@ -3131,7 +3148,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" s="3">
         <v>5</v>
@@ -3154,7 +3171,7 @@
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="3">
         <v>2</v>
@@ -3163,7 +3180,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="3">
         <v>5</v>
@@ -3186,7 +3203,7 @@
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" s="3">
         <v>3</v>
@@ -3195,7 +3212,7 @@
         <v>5</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E26" s="3">
         <v>4</v>
@@ -3241,9 +3258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3276,11 +3293,11 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3300,44 +3317,44 @@
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
+      <c r="C6" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>3</v>
+      <c r="E6" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>3</v>
+      <c r="G6" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
@@ -3360,7 +3377,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="5">
         <v>5</v>
@@ -3383,7 +3400,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="5">
         <v>5</v>
@@ -3406,7 +3423,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="5">
         <v>5</v>
@@ -3429,7 +3446,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="5">
         <v>5</v>
@@ -3452,7 +3469,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" s="5">
         <v>5</v>
@@ -3475,7 +3492,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" s="5">
         <v>5</v>
@@ -3498,7 +3515,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" s="5">
         <v>3</v>
@@ -3521,7 +3538,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15" s="5">
         <v>5</v>
@@ -3544,7 +3561,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="5">
         <v>5</v>
@@ -3567,7 +3584,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="5">
         <v>5</v>
@@ -3590,7 +3607,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="5">
         <v>5</v>
@@ -3613,7 +3630,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="5">
         <v>5</v>
@@ -3636,7 +3653,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="5">
         <v>5</v>
@@ -3659,7 +3676,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="5">
         <v>5</v>
@@ -3682,7 +3699,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="5">
         <v>0</v>
@@ -3705,7 +3722,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B23" s="3">
         <v>3</v>
@@ -3728,7 +3745,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B24" s="5">
         <v>3</v>
@@ -3751,7 +3768,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" s="5">
         <v>4</v>
@@ -3774,7 +3791,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B26" s="5">
         <v>5</v>

</xml_diff>